<commit_message>
Fixed footsteps/jetpack and implemented jetpack
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{28DC2DB0-0F7E-4CFD-A865-9EF1FBE13FD7}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6245D7A7-D8FF-4FC0-B492-02AB03D4AC02}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
   <si>
     <t>Event</t>
   </si>
@@ -292,9 +292,6 @@
   </si>
   <si>
     <t>Revising</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
   <si>
     <t>Completed</t>
@@ -882,7 +879,7 @@
         <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented drone hovering sound
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9C2BFE5F-8A04-4513-B3B8-0AF7892D5FA6}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A199A623-C15D-4C3C-88AB-1A655D91DF84}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="82">
   <si>
     <t>Event</t>
   </si>
@@ -600,7 +600,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,6 +688,9 @@
       <c r="D5" t="s">
         <v>62</v>
       </c>
+      <c r="E5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
Added weapon swap sound
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A199A623-C15D-4C3C-88AB-1A655D91DF84}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B55F6CB8-3B5A-4B72-B1D7-4CB78A62C0FC}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
   <si>
     <t>Event</t>
   </si>
@@ -600,7 +600,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,6 +818,9 @@
       <c r="D13" t="s">
         <v>34</v>
       </c>
+      <c r="E13" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
Implemented turret alert sound
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B55F6CB8-3B5A-4B72-B1D7-4CB78A62C0FC}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{355424F1-5171-4B7D-8290-4497AFB1344D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
   <si>
     <t>Event</t>
   </si>
@@ -243,9 +243,6 @@
     <t>Ambience of the wind and lava below</t>
   </si>
   <si>
-    <t>Wind loop SFX (x2), Lava bubbling SFX (x3)</t>
-  </si>
-  <si>
     <t>Death</t>
   </si>
   <si>
@@ -271,6 +268,9 @@
   </si>
   <si>
     <t>In progress</t>
+  </si>
+  <si>
+    <t>Wind loop SFX (x2), Lava bubbling SFX</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,7 +630,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -705,6 +705,9 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -748,10 +751,10 @@
         <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -765,13 +768,13 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -788,7 +791,7 @@
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -819,7 +822,7 @@
         <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -864,7 +867,7 @@
         <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -880,6 +883,9 @@
       <c r="D17" t="s">
         <v>49</v>
       </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -895,7 +901,7 @@
         <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -912,7 +918,7 @@
         <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -943,7 +949,7 @@
         <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -962,16 +968,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
         <v>73</v>
-      </c>
-      <c r="B23" t="s">
-        <v>74</v>
       </c>
       <c r="C23" t="s">
         <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -988,7 +994,7 @@
         <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1002,10 +1008,10 @@
         <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented objective notification sound
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{355424F1-5171-4B7D-8290-4497AFB1344D}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0CF8282D-FE71-4621-B252-0267EDD09D92}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
   <si>
     <t>Event</t>
   </si>
@@ -600,7 +600,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,6 +838,9 @@
       <c r="D14" t="s">
         <v>37</v>
       </c>
+      <c r="E14" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">

</xml_diff>

<commit_message>
Added objective complete sound
Also modified ambience to be lower volume
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="184" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0CF8282D-FE71-4621-B252-0267EDD09D92}"/>
+  <xr:revisionPtr revIDLastSave="190" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C2A6474D-B3B7-4AC8-91DD-0CE452C90394}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="86">
   <si>
     <t>Event</t>
   </si>
@@ -271,6 +271,18 @@
   </si>
   <si>
     <t>Wind loop SFX (x2), Lava bubbling SFX</t>
+  </si>
+  <si>
+    <t>Steven: Might be a bit too much of a funny sound</t>
+  </si>
+  <si>
+    <t>Steven: A bit more bass</t>
+  </si>
+  <si>
+    <t>Steven: Might need higher frequency or layer (blends in too much)</t>
+  </si>
+  <si>
+    <t>Revised per Steven's feedback</t>
   </si>
 </sst>
 </file>
@@ -600,7 +612,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,6 +703,9 @@
       <c r="E5" t="s">
         <v>79</v>
       </c>
+      <c r="F5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -824,6 +839,9 @@
       <c r="E13" t="s">
         <v>79</v>
       </c>
+      <c r="F13" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -855,6 +873,9 @@
       <c r="D15" t="s">
         <v>37</v>
       </c>
+      <c r="E15" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -873,7 +894,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -890,7 +911,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -907,7 +928,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -923,8 +944,11 @@
       <c r="E19" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -938,7 +962,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -955,7 +979,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -969,7 +993,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -983,7 +1007,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -1000,7 +1024,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -1015,6 +1039,9 @@
       </c>
       <c r="E25" t="s">
         <v>79</v>
+      </c>
+      <c r="F25" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added hoverbot and turret attack sounds
Had some others that I scrapped cause they sounded bad in-game
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C2A6474D-B3B7-4AC8-91DD-0CE452C90394}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DBB75A64-95B8-40A8-A528-B76D73589040}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="86">
   <si>
     <t>Event</t>
   </si>
@@ -612,7 +612,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,6 +672,9 @@
       <c r="D3" t="s">
         <v>47</v>
       </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -736,6 +739,9 @@
       </c>
       <c r="D7" t="s">
         <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented health pickup sound
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="192" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DBB75A64-95B8-40A8-A528-B76D73589040}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{579ED540-214A-418D-8144-3B8FB9568FB6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="86">
   <si>
     <t>Event</t>
   </si>
@@ -225,9 +225,6 @@
     <t>Sound of the player replenishing health</t>
   </si>
   <si>
-    <t>Health increase SFX (x2)</t>
-  </si>
-  <si>
     <t>LowHealth</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>Revised per Steven's feedback</t>
+  </si>
+  <si>
+    <t>Health increase SFX</t>
   </si>
 </sst>
 </file>
@@ -612,7 +612,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
         <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -704,10 +704,10 @@
         <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -741,7 +741,7 @@
         <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -772,10 +772,10 @@
         <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -789,13 +789,13 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -812,7 +812,7 @@
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -843,10 +843,10 @@
         <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -863,7 +863,7 @@
         <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
         <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -897,7 +897,7 @@
         <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -914,7 +914,7 @@
         <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -931,7 +931,7 @@
         <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -948,10 +948,10 @@
         <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -982,7 +982,7 @@
         <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -996,58 +996,61 @@
         <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>85</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
         <v>72</v>
-      </c>
-      <c r="B23" t="s">
-        <v>73</v>
       </c>
       <c r="C23" t="s">
         <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
         <v>67</v>
-      </c>
-      <c r="B24" t="s">
-        <v>68</v>
       </c>
       <c r="C24" t="s">
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
         <v>70</v>
       </c>
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented turret death sound
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{579ED540-214A-418D-8144-3B8FB9568FB6}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FDE43FA1-0FE3-4C76-B6A5-61BC732BC6FF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="86">
   <si>
     <t>Event</t>
   </si>
@@ -612,7 +612,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,6 +757,9 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
+      <c r="E8" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">

</xml_diff>

<commit_message>
Hoverbot alert sound implemented
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FDE43FA1-0FE3-4C76-B6A5-61BC732BC6FF}"/>
+  <xr:revisionPtr revIDLastSave="197" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D21F9270-6AD2-4568-A326-A2FAA3DF9B6E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
   <si>
     <t>Event</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>Health increase SFX</t>
+  </si>
+  <si>
+    <t>Might need to be made a bit more hostile sounding</t>
   </si>
 </sst>
 </file>
@@ -612,7 +615,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,6 +661,12 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Added weapon damage tick noise
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4682269C-467E-4678-8D01-B2D7A1FA8022}"/>
+  <xr:revisionPtr revIDLastSave="200" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A357F6E1-4991-4B7D-A08E-603025602D93}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
   <si>
     <t>Event</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>Might need to be made a bit more hostile sounding</t>
+  </si>
+  <si>
+    <t>May need to be a bit more crisp sounding</t>
   </si>
 </sst>
 </file>
@@ -615,7 +618,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,6 +843,12 @@
       <c r="D12" t="s">
         <v>59</v>
       </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">

</xml_diff>

<commit_message>
Implemented hoverbot death sound
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A357F6E1-4991-4B7D-A08E-603025602D93}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B8DF09BC-D7A8-4E35-BDD3-B43FB9267EDB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
   <si>
     <t>Event</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>May need to be a bit more crisp sounding</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
   </si>
 </sst>
 </file>
@@ -618,7 +621,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,6 +704,9 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
+      <c r="E4" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -987,6 +993,9 @@
       </c>
       <c r="D20" t="s">
         <v>58</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Set up low health and created click/hover sounds
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B8DF09BC-D7A8-4E35-BDD3-B43FB9267EDB}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0EEFECEF-BCC4-4416-AE09-93EE10575C6B}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="95">
   <si>
     <t>Event</t>
   </si>
@@ -292,6 +292,24 @@
   </si>
   <si>
     <t>Incomplete</t>
+  </si>
+  <si>
+    <t>UIClick</t>
+  </si>
+  <si>
+    <t>UIHover</t>
+  </si>
+  <si>
+    <t>Sound of clicking on a button</t>
+  </si>
+  <si>
+    <t>Sound of hovering over a button</t>
+  </si>
+  <si>
+    <t>Click SFX (x2)</t>
+  </si>
+  <si>
+    <t>Hover SFX (x2)</t>
   </si>
 </sst>
 </file>
@@ -618,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1081,7 @@
         <v>68</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1084,6 +1102,40 @@
       </c>
       <c r="F25" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added UI sounds and damage sound
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0EEFECEF-BCC4-4416-AE09-93EE10575C6B}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{39050868-5A67-448B-874A-99DECD15AF82}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="96">
   <si>
     <t>Event</t>
   </si>
@@ -201,9 +201,6 @@
     <t>Sound of the player taking damage</t>
   </si>
   <si>
-    <t>Damage SFX (x3)</t>
-  </si>
-  <si>
     <t>Damage tick SFX (x2)</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>Wind loop SFX (x2), Lava bubbling SFX</t>
   </si>
   <si>
@@ -291,9 +285,6 @@
     <t>May need to be a bit more crisp sounding</t>
   </si>
   <si>
-    <t>Incomplete</t>
-  </si>
-  <si>
     <t>UIClick</t>
   </si>
   <si>
@@ -310,6 +301,18 @@
   </si>
   <si>
     <t>Hover SFX (x2)</t>
+  </si>
+  <si>
+    <t>Damage SFX (x2)</t>
+  </si>
+  <si>
+    <t>UIDrag</t>
+  </si>
+  <si>
+    <t>Sound of a slider being dragged</t>
+  </si>
+  <si>
+    <t>Drag SFX (x2)</t>
   </si>
 </sst>
 </file>
@@ -636,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +672,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -686,10 +689,10 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -706,7 +709,7 @@
         <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -723,7 +726,7 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -737,13 +740,13 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -760,7 +763,7 @@
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -777,7 +780,7 @@
         <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -794,7 +797,7 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -811,10 +814,10 @@
         <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -828,13 +831,13 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -851,7 +854,7 @@
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -865,13 +868,13 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -888,10 +891,10 @@
         <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -908,7 +911,7 @@
         <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -925,7 +928,7 @@
         <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -942,7 +945,7 @@
         <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -959,7 +962,7 @@
         <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -976,7 +979,7 @@
         <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -993,10 +996,10 @@
         <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1010,132 +1013,149 @@
         <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
         <v>60</v>
-      </c>
-      <c r="B21" t="s">
-        <v>61</v>
       </c>
       <c r="C21" t="s">
         <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
         <v>64</v>
-      </c>
-      <c r="B22" t="s">
-        <v>65</v>
       </c>
       <c r="C22" t="s">
         <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
         <v>71</v>
-      </c>
-      <c r="B23" t="s">
-        <v>72</v>
       </c>
       <c r="C23" t="s">
         <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
         <v>66</v>
-      </c>
-      <c r="B24" t="s">
-        <v>67</v>
       </c>
       <c r="C24" t="s">
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
         <v>69</v>
       </c>
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
         <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
         <v>33</v>
       </c>
       <c r="D27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
         <v>94</v>
       </c>
-      <c r="E27" t="s">
-        <v>79</v>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited heavy landing sound
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8f0220009ecbd109/School Work/Interactive Audio/FinalProject/671-Final-Project/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{39050868-5A67-448B-874A-99DECD15AF82}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="11_F25DC773A252ABDACC1048B719D9552A5BDE58E4" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4075642A-FBF9-4C50-A416-6468A3B5DFE0}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="95">
   <si>
     <t>Event</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>Wind loop SFX (x2), Lava bubbling SFX</t>
-  </si>
-  <si>
-    <t>Steven: Might be a bit too much of a funny sound</t>
   </si>
   <si>
     <t>Steven: A bit more bass</t>
@@ -641,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +689,7 @@
         <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -746,7 +743,7 @@
         <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -874,7 +871,7 @@
         <v>77</v>
       </c>
       <c r="F12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -894,7 +891,7 @@
         <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -999,7 +996,7 @@
         <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1013,7 +1010,7 @@
         <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E20" t="s">
         <v>77</v>
@@ -1047,7 +1044,7 @@
         <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E22" t="s">
         <v>77</v>
@@ -1104,21 +1101,21 @@
         <v>77</v>
       </c>
       <c r="F25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
         <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E26" t="s">
         <v>77</v>
@@ -1126,16 +1123,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
         <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E27" t="s">
         <v>77</v>
@@ -1143,16 +1140,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" t="s">
         <v>93</v>
-      </c>
-      <c r="B28" t="s">
-        <v>94</v>
       </c>
       <c r="C28" t="s">
         <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E28" t="s">
         <v>77</v>

</xml_diff>